<commit_message>
Finished all Login testing, trouble shooting still needed for tests
</commit_message>
<xml_diff>
--- a/Documentation/Java_Test_Plan/bug_report.xlsx
+++ b/Documentation/Java_Test_Plan/bug_report.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Danny\Desktop\The-Jungle-2\Documentation\Java_Test_Plan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{85B05821-B41A-4C06-9F76-57D541615166}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D1CD423-5EA8-4DA5-80BB-05DE786A8ED7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2910" windowWidth="21600" windowHeight="11835" xr2:uid="{A257C043-C230-457B-A571-9896D12BE7EE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{A257C043-C230-457B-A571-9896D12BE7EE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -608,7 +608,7 @@
   <dimension ref="A1:N6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="A3:G4"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -675,6 +675,9 @@
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
       <c r="K3" s="1" t="s">
         <v>7</v>
       </c>

</xml_diff>